<commit_message>
chaging EL faqs and updating data sources
</commit_message>
<xml_diff>
--- a/src/assets/ChatTrinityDramaSourceData.xlsx
+++ b/src/assets/ChatTrinityDramaSourceData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Vivo Music Dropbox\Trinity College London\TCL National\Strategy &amp; R&amp;D\R&amp;D\Chatbot\Source Data\Drama\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Vivo Music Dropbox\Trinity College London\TCL National\Strategy &amp; R&amp;D\R&amp;D\Chatbot\Code\ChatTrinity\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA66391-D08A-44EA-967A-F23088E6698D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E148F2A-04EF-46F0-BE1A-7B690B1DC5CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{767CB8E1-717A-4A4B-9A2F-73181A3DE1DB}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="80">
   <si>
     <t>Web/PDF</t>
   </si>
@@ -265,13 +265,16 @@
   </si>
   <si>
     <t>PDF</t>
+  </si>
+  <si>
+    <t>https://www.trinitycollege.com/about-us/work-with-trinity/registered-exam-centre</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,6 +286,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -305,14 +316,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -625,7 +639,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C14BDF-EED2-4551-A2A9-086DD03AE42C}">
-  <dimension ref="A1:B76"/>
+  <dimension ref="A1:B77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1005,10 +1019,10 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>78</v>
-      </c>
-      <c r="B47" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.45">
@@ -1016,7 +1030,7 @@
         <v>78</v>
       </c>
       <c r="B48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.45">
@@ -1024,7 +1038,7 @@
         <v>78</v>
       </c>
       <c r="B49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.45">
@@ -1032,7 +1046,7 @@
         <v>78</v>
       </c>
       <c r="B50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.45">
@@ -1040,7 +1054,7 @@
         <v>78</v>
       </c>
       <c r="B51" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.45">
@@ -1048,7 +1062,7 @@
         <v>78</v>
       </c>
       <c r="B52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.45">
@@ -1056,7 +1070,7 @@
         <v>78</v>
       </c>
       <c r="B53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.45">
@@ -1064,7 +1078,7 @@
         <v>78</v>
       </c>
       <c r="B54" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.45">
@@ -1072,7 +1086,7 @@
         <v>78</v>
       </c>
       <c r="B55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.45">
@@ -1080,7 +1094,7 @@
         <v>78</v>
       </c>
       <c r="B56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.45">
@@ -1088,7 +1102,7 @@
         <v>78</v>
       </c>
       <c r="B57" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.45">
@@ -1096,7 +1110,7 @@
         <v>78</v>
       </c>
       <c r="B58" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.45">
@@ -1104,7 +1118,7 @@
         <v>78</v>
       </c>
       <c r="B59" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.45">
@@ -1112,7 +1126,7 @@
         <v>78</v>
       </c>
       <c r="B60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.45">
@@ -1120,7 +1134,7 @@
         <v>78</v>
       </c>
       <c r="B61" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.45">
@@ -1128,7 +1142,7 @@
         <v>78</v>
       </c>
       <c r="B62" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.45">
@@ -1136,7 +1150,7 @@
         <v>78</v>
       </c>
       <c r="B63" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.45">
@@ -1144,7 +1158,7 @@
         <v>78</v>
       </c>
       <c r="B64" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.45">
@@ -1152,7 +1166,7 @@
         <v>78</v>
       </c>
       <c r="B65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.45">
@@ -1160,7 +1174,7 @@
         <v>78</v>
       </c>
       <c r="B66" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.45">
@@ -1168,7 +1182,7 @@
         <v>78</v>
       </c>
       <c r="B67" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.45">
@@ -1176,7 +1190,7 @@
         <v>78</v>
       </c>
       <c r="B68" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.45">
@@ -1184,7 +1198,7 @@
         <v>78</v>
       </c>
       <c r="B69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.45">
@@ -1192,7 +1206,7 @@
         <v>78</v>
       </c>
       <c r="B70" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.45">
@@ -1200,7 +1214,7 @@
         <v>78</v>
       </c>
       <c r="B71" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.45">
@@ -1208,7 +1222,7 @@
         <v>78</v>
       </c>
       <c r="B72" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.45">
@@ -1216,7 +1230,7 @@
         <v>78</v>
       </c>
       <c r="B73" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.45">
@@ -1224,7 +1238,7 @@
         <v>78</v>
       </c>
       <c r="B74" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.45">
@@ -1232,7 +1246,7 @@
         <v>78</v>
       </c>
       <c r="B75" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.45">
@@ -1240,11 +1254,22 @@
         <v>78</v>
       </c>
       <c r="B76" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
+        <v>78</v>
+      </c>
+      <c r="B77" t="s">
         <v>77</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B1" xr:uid="{50C14BDF-EED2-4551-A2A9-086DD03AE42C}"/>
+  <hyperlinks>
+    <hyperlink ref="B47" r:id="rId1" xr:uid="{ABD2C9E8-B835-414A-A865-FE6565F999BE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update drama data sources
</commit_message>
<xml_diff>
--- a/src/assets/ChatTrinityDramaSourceData.xlsx
+++ b/src/assets/ChatTrinityDramaSourceData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Vivo Music Dropbox\Trinity College London\TCL National\Strategy &amp; R&amp;D\R&amp;D\Chatbot\Code\ChatTrinity\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E148F2A-04EF-46F0-BE1A-7B690B1DC5CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F227FC94-6A14-4C38-B230-8D7B6C9B4051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{767CB8E1-717A-4A4B-9A2F-73181A3DE1DB}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="81">
   <si>
     <t>Web/PDF</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>https://www.trinitycollege.com/about-us/work-with-trinity/registered-exam-centre</t>
+  </si>
+  <si>
+    <t>https://www.trinitycollege.com/qualifications/drama/certificates/performance-certificates</t>
   </si>
 </sst>
 </file>
@@ -639,7 +642,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C14BDF-EED2-4551-A2A9-086DD03AE42C}">
-  <dimension ref="A1:B77"/>
+  <dimension ref="A1:B78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -659,242 +662,242 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B27" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
@@ -902,7 +905,7 @@
         <v>47</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
@@ -910,7 +913,7 @@
         <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
@@ -918,7 +921,7 @@
         <v>47</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.45">
@@ -926,7 +929,7 @@
         <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.45">
@@ -934,7 +937,7 @@
         <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
@@ -942,7 +945,7 @@
         <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
@@ -950,7 +953,7 @@
         <v>47</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.45">
@@ -958,7 +961,7 @@
         <v>47</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.45">
@@ -966,7 +969,7 @@
         <v>47</v>
       </c>
       <c r="B40" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
@@ -974,7 +977,7 @@
         <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.45">
@@ -982,7 +985,7 @@
         <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.45">
@@ -990,7 +993,7 @@
         <v>47</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.45">
@@ -998,7 +1001,7 @@
         <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.45">
@@ -1006,7 +1009,7 @@
         <v>47</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.45">
@@ -1014,261 +1017,273 @@
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>79</v>
+      <c r="B47" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B51" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B52" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B53" t="s">
-        <v>53</v>
+        <v>23</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B54" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B55" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B56" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B57" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B58" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B59" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B60" t="s">
-        <v>60</v>
+        <v>30</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B61" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B62" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B63" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B64" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B65" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B66" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B67" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B68" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B69" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>78</v>
-      </c>
-      <c r="B70" t="s">
-        <v>70</v>
+        <v>47</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B71" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B72" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B73" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B74" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B75" t="s">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B76" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B77" t="s">
-        <v>77</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
+        <v>47</v>
+      </c>
+      <c r="B78" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:B1" xr:uid="{50C14BDF-EED2-4551-A2A9-086DD03AE42C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B78">
+    <sortCondition ref="A2:A78"/>
+    <sortCondition ref="B2:B78"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="B47" r:id="rId1" xr:uid="{ABD2C9E8-B835-414A-A865-FE6565F999BE}"/>
+    <hyperlink ref="B70" r:id="rId1" xr:uid="{ABD2C9E8-B835-414A-A865-FE6565F999BE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated source data files
</commit_message>
<xml_diff>
--- a/src/assets/ChatTrinityDramaSourceData.xlsx
+++ b/src/assets/ChatTrinityDramaSourceData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Vivo Music Dropbox\Trinity College London\TCL National\Strategy &amp; R&amp;D\R&amp;D\Chatbot\Code\ChatTrinity\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F227FC94-6A14-4C38-B230-8D7B6C9B4051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4015AE-B7E0-4DFF-A987-12F566F7B0E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{767CB8E1-717A-4A4B-9A2F-73181A3DE1DB}"/>
   </bookViews>
@@ -23,12 +23,23 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="82">
   <si>
     <t>Web/PDF</t>
   </si>
@@ -271,6 +282,9 @@
   </si>
   <si>
     <t>https://www.trinitycollege.com/qualifications/drama/certificates/performance-certificates</t>
+  </si>
+  <si>
+    <t>https://www.trinitycollege.com/local-trinity/UK/drama-speech-dance/exam-help</t>
   </si>
 </sst>
 </file>
@@ -642,9 +656,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C14BDF-EED2-4551-A2A9-086DD03AE42C}">
-  <dimension ref="A1:B78"/>
+  <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1274,6 +1290,14 @@
       </c>
       <c r="B78" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A79" t="s">
+        <v>47</v>
+      </c>
+      <c r="B79" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>